<commit_message>
added form for insurance
</commit_message>
<xml_diff>
--- a/koboforms/section3.xlsx
+++ b/koboforms/section3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deo/generateKobo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deo/whatsthepointgameinteractive/koboforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3506D77-1D48-F147-AF5D-7158E99E0150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA52978-483A-CF40-B541-4581109958F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32500" yWindow="-22380" windowWidth="28040" windowHeight="17440" xr2:uid="{05574417-E28B-7A44-8D51-6FA488FA6DA5}"/>
+    <workbookView xWindow="4560" yWindow="-17740" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{05574417-E28B-7A44-8D51-6FA488FA6DA5}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
   <si>
     <t>type</t>
   </si>
@@ -51,58 +51,79 @@
     <t>text</t>
   </si>
   <si>
-    <t>select_one yes_no</t>
+    <t>invest</t>
+  </si>
+  <si>
+    <t>Do you want to invest?</t>
+  </si>
+  <si>
+    <t>list_name</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>form_title</t>
+  </si>
+  <si>
+    <t>form_id</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>v1</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>required</t>
+  </si>
+  <si>
+    <t>select_one invest_options</t>
+  </si>
+  <si>
+    <t>invest_choice</t>
+  </si>
+  <si>
+    <t>invest_options</t>
+  </si>
+  <si>
+    <t>Invest</t>
+  </si>
+  <si>
+    <t>dont_invest</t>
+  </si>
+  <si>
+    <t>Don’t Invest</t>
+  </si>
+  <si>
+    <t>WhatsThePointGameInteractive_Section1</t>
+  </si>
+  <si>
+    <t>Your email</t>
+  </si>
+  <si>
+    <t>Do you want to buy insurance?</t>
+  </si>
+  <si>
+    <t>insurance_choice</t>
+  </si>
+  <si>
+    <t>buy_insurance</t>
+  </si>
+  <si>
+    <t>Buy Insurance</t>
+  </si>
+  <si>
+    <t>dont_buyInsurance</t>
+  </si>
+  <si>
+    <t>Dont buy Insurance</t>
   </si>
   <si>
     <t>section3</t>
-  </si>
-  <si>
-    <t>regret</t>
-  </si>
-  <si>
-    <t>Do you regret your choice?</t>
-  </si>
-  <si>
-    <t>list_name</t>
-  </si>
-  <si>
-    <t>yes_no</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>form_title</t>
-  </si>
-  <si>
-    <t>form_id</t>
-  </si>
-  <si>
-    <t>version</t>
-  </si>
-  <si>
-    <t>v1</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>required</t>
-  </si>
-  <si>
-    <t>WhatsThePointGameInteractive_Section3</t>
-  </si>
-  <si>
-    <t>Your email</t>
   </si>
 </sst>
 </file>
@@ -463,14 +484,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{994C7F9E-9867-6243-AAB9-77628DC2993D}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="32.1640625" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
   </cols>
   <sheetData>
@@ -485,7 +507,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -493,27 +515,41 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
         <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
-        <v>10</v>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -523,17 +559,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B613F314-F1A9-E94C-8850-BA4A407A86FF}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -544,24 +583,46 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -573,24 +634,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8DF2FC2-2B0D-0B42-899E-2C094C966549}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17.33203125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -598,10 +656,10 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modern response figures, starting insurance and invest
</commit_message>
<xml_diff>
--- a/koboforms/section3.xlsx
+++ b/koboforms/section3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deo/whatsthepointgameinteractive/koboforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA52978-483A-CF40-B541-4581109958F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C11AE5AA-99B9-E444-B95A-D508BACE179A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4560" yWindow="-17740" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{05574417-E28B-7A44-8D51-6FA488FA6DA5}"/>
+    <workbookView xWindow="4560" yWindow="-17740" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{05574417-E28B-7A44-8D51-6FA488FA6DA5}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>type</t>
   </si>
@@ -124,6 +124,12 @@
   </si>
   <si>
     <t>section3</t>
+  </si>
+  <si>
+    <t>select_one insurance_options</t>
+  </si>
+  <si>
+    <t>insurance_options</t>
   </si>
 </sst>
 </file>
@@ -487,11 +493,12 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="26" customWidth="1"/>
     <col min="2" max="2" width="32.1640625" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
   </cols>
@@ -540,7 +547,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
         <v>23</v>
@@ -561,8 +568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B613F314-F1A9-E94C-8850-BA4A407A86FF}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -605,7 +612,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
         <v>24</v>
@@ -616,7 +623,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
         <v>26</v>
@@ -634,7 +641,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8DF2FC2-2B0D-0B42-899E-2C094C966549}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>